<commit_message>
fix bug in sales subtraction
</commit_message>
<xml_diff>
--- a/results/COVID Budget Impact Analysis (March 2021).xlsx
+++ b/results/COVID Budget Impact Analysis (March 2021).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholashand/LocalWork/Projects/BudgetWork/Analysis/v2/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholashand/Software/covid19-forecaster/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3423660-3A39-BD46-BE8E-B0358DCDCCB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBC808D-C38F-0344-99A9-04402BB67206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1612,7 +1612,7 @@
   <dimension ref="B3:J28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
@@ -1864,36 +1864,36 @@
         <v>14</v>
       </c>
       <c r="C13" s="93">
-        <f>'Budget Revenues'!C7 - C27</f>
-        <v>173876.16655304801</v>
+        <f>'Budget Revenues'!C7 - C26</f>
+        <v>174507.81655304797</v>
       </c>
       <c r="D13" s="94">
-        <f>'Optimistic (Raw)'!C7 - C27</f>
-        <v>205342.3913346809</v>
+        <f>'Optimistic (Raw)'!C7 - C26</f>
+        <v>205974.04133468086</v>
       </c>
       <c r="E13" s="55">
-        <f>'Pessimistic (Raw)'!C7 - C27</f>
-        <v>201019.97437850229</v>
+        <f>'Pessimistic (Raw)'!C7 - C26</f>
+        <v>201651.62437850225</v>
       </c>
       <c r="F13" s="95">
-        <f>'Budget Revenues'!E7 - C28</f>
-        <v>315121.01426197897</v>
+        <f>'Budget Revenues'!E7 - C27</f>
+        <v>198598.55626197899</v>
       </c>
       <c r="G13" s="94">
-        <f>'Optimistic (Raw)'!D7 - C28</f>
-        <v>339683.71317785408</v>
+        <f>'Optimistic (Raw)'!D7 - C27</f>
+        <v>223161.25517785409</v>
       </c>
       <c r="H13" s="56">
-        <f>'Pessimistic (Raw)'!D7 - C28</f>
-        <v>328491.53624475643</v>
+        <f>'Pessimistic (Raw)'!D7 - C27</f>
+        <v>211969.07824475644</v>
       </c>
       <c r="I13" s="88">
         <f t="shared" si="0"/>
-        <v>56028.923697508057</v>
+        <v>56028.923697507998</v>
       </c>
       <c r="J13" s="53">
         <f t="shared" si="1"/>
-        <v>40514.329808231792</v>
+        <v>40514.329808231734</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="20" customHeight="1">
@@ -2050,35 +2050,35 @@
       </c>
       <c r="C18" s="96">
         <f t="shared" ref="C18:J18" si="2">SUM(C9:C17)</f>
-        <v>3831257.166553048</v>
+        <v>3831888.8165530479</v>
       </c>
       <c r="D18" s="97">
         <f t="shared" si="2"/>
-        <v>3887290.9096506694</v>
+        <v>3887922.5596506693</v>
       </c>
       <c r="E18" s="62">
         <f t="shared" si="2"/>
-        <v>3808044.4067889079</v>
+        <v>3808676.0567889079</v>
       </c>
       <c r="F18" s="63">
         <f t="shared" si="2"/>
-        <v>4370181.5315734008</v>
+        <v>4253659.0735734012</v>
       </c>
       <c r="G18" s="64">
         <f t="shared" si="2"/>
-        <v>4281233.749577729</v>
+        <v>4164711.2915777303</v>
       </c>
       <c r="H18" s="65">
         <f t="shared" si="2"/>
-        <v>4109742.0283255558</v>
+        <v>3993219.5703255557</v>
       </c>
       <c r="I18" s="98">
         <f t="shared" si="2"/>
-        <v>-32914.03889804917</v>
+        <v>-32914.038898049228</v>
       </c>
       <c r="J18" s="66">
         <f t="shared" si="2"/>
-        <v>-283652.26301198435</v>
+        <v>-283652.26301198447</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="20" customHeight="1">

</xml_diff>